<commit_message>
bf: add some forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Burkina Faso/2023 may/bf_202305_sch_impact_assessment_1_sites.xlsx
+++ b/SCH-STH/Impact assessments/Burkina Faso/2023 may/bf_202305_sch_impact_assessment_1_sites.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Burkina Faso\2023 may\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0405A126-1B25-4BEA-9984-6066DD25B788}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2654CAD-D5AF-494A-B19E-3D26A0A99BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="288">
   <si>
     <t>type</t>
   </si>
@@ -351,252 +363,9 @@
     <t>EN08</t>
   </si>
   <si>
-    <t>Centre</t>
-  </si>
-  <si>
-    <t>Hauts Bassins</t>
-  </si>
-  <si>
-    <t>Sud-Ouest</t>
-  </si>
-  <si>
-    <t>Bogodogo</t>
-  </si>
-  <si>
-    <t>Boulmiougou</t>
-  </si>
-  <si>
-    <t>Do</t>
-  </si>
-  <si>
-    <t>Lena</t>
-  </si>
-  <si>
-    <t>Karangasso-vigue</t>
-  </si>
-  <si>
-    <t>N'Dorola</t>
-  </si>
-  <si>
-    <t>Diebougou</t>
-  </si>
-  <si>
-    <t>Diébougou</t>
-  </si>
-  <si>
-    <t>DIDRI</t>
-  </si>
-  <si>
-    <t>KOUBRI</t>
-  </si>
-  <si>
-    <t>PIKIEKO</t>
-  </si>
-  <si>
-    <t>TANVINAKAMTENGA</t>
-  </si>
-  <si>
-    <t>TANVI-NAKAMTENGA</t>
-  </si>
-  <si>
-    <t>CMSAABA</t>
-  </si>
-  <si>
-    <t>CM SAABA</t>
-  </si>
-  <si>
-    <t>GAMPELA</t>
-  </si>
-  <si>
-    <t>KOALA</t>
-  </si>
-  <si>
-    <t>NIOKO1</t>
-  </si>
-  <si>
-    <t>NIOKO 1</t>
-  </si>
-  <si>
-    <t>TANLARGHIN</t>
-  </si>
-  <si>
-    <t>WENDEFANDE</t>
-  </si>
-  <si>
-    <t>WENDE FANDE</t>
-  </si>
-  <si>
-    <t>TINTILOUSUD</t>
-  </si>
-  <si>
-    <t>TINTILOU SUD</t>
-  </si>
-  <si>
-    <t>BASSEMYAM</t>
-  </si>
-  <si>
-    <t>KIENFANGUE</t>
-  </si>
-  <si>
-    <t>PONSMTENGA</t>
-  </si>
-  <si>
-    <t>ZEGUEDESSE</t>
-  </si>
-  <si>
     <t>BOULSIN</t>
   </si>
   <si>
-    <t>BOULSIN (OUAGA)</t>
-  </si>
-  <si>
-    <t>CM DASSOURI</t>
-  </si>
-  <si>
-    <t>KOUDIERE</t>
-  </si>
-  <si>
-    <t>SANE</t>
-  </si>
-  <si>
-    <t>YIMDI</t>
-  </si>
-  <si>
-    <t>DOGONA</t>
-  </si>
-  <si>
-    <t>KIRI</t>
-  </si>
-  <si>
-    <t>KOUMI</t>
-  </si>
-  <si>
-    <t>NASSO</t>
-  </si>
-  <si>
-    <t>BOUENDE</t>
-  </si>
-  <si>
-    <t>KSAMBLA</t>
-  </si>
-  <si>
-    <t>K SAMBLA</t>
-  </si>
-  <si>
-    <t>MARBAGASSO</t>
-  </si>
-  <si>
-    <t>PENI</t>
-  </si>
-  <si>
-    <t>TAPOKO</t>
-  </si>
-  <si>
-    <t>TOUSSIANA</t>
-  </si>
-  <si>
-    <t>DAN</t>
-  </si>
-  <si>
-    <t>DEGUELIN</t>
-  </si>
-  <si>
-    <t>DIOSSO</t>
-  </si>
-  <si>
-    <t>KVIGUE</t>
-  </si>
-  <si>
-    <t>POYA</t>
-  </si>
-  <si>
-    <t>SOUMOUSSO</t>
-  </si>
-  <si>
-    <t>WARA</t>
-  </si>
-  <si>
-    <t>YEGUERE</t>
-  </si>
-  <si>
-    <t>BAH</t>
-  </si>
-  <si>
-    <t>KOFILA</t>
-  </si>
-  <si>
-    <t>LENA</t>
-  </si>
-  <si>
-    <t>BALA</t>
-  </si>
-  <si>
-    <t>BOSSORA</t>
-  </si>
-  <si>
-    <t>DEFINA</t>
-  </si>
-  <si>
-    <t>KADOMBA</t>
-  </si>
-  <si>
-    <t>KOROMA</t>
-  </si>
-  <si>
-    <t>SATIRI</t>
-  </si>
-  <si>
-    <t>TIARAKO</t>
-  </si>
-  <si>
-    <t>KOKORO</t>
-  </si>
-  <si>
-    <t>KOUROUMA</t>
-  </si>
-  <si>
-    <t>SADINA</t>
-  </si>
-  <si>
-    <t>FADONA</t>
-  </si>
-  <si>
-    <t>N'DOROLA</t>
-  </si>
-  <si>
-    <t>SILOROLA</t>
-  </si>
-  <si>
-    <t>BAMAKO</t>
-  </si>
-  <si>
-    <t>BAPLA</t>
-  </si>
-  <si>
-    <t>BONDIGUI</t>
-  </si>
-  <si>
-    <t>COMMUNAL</t>
-  </si>
-  <si>
-    <t>DANKOBLE</t>
-  </si>
-  <si>
-    <t>DOLO</t>
-  </si>
-  <si>
-    <t>KONSABLA</t>
-  </si>
-  <si>
-    <t>NABERE</t>
-  </si>
-  <si>
-    <t>POKOURO</t>
-  </si>
-  <si>
-    <t>TIOYO</t>
-  </si>
-  <si>
     <t>OuiNon_list</t>
   </si>
   <si>
@@ -879,29 +648,266 @@
     <t>French</t>
   </si>
   <si>
-    <t>Fara</t>
-  </si>
-  <si>
-    <t>Foulasso</t>
-  </si>
-  <si>
-    <t>Kodona</t>
-  </si>
-  <si>
-    <t>Seguedougou</t>
-  </si>
-  <si>
-    <t>(BF - Jan 2023) impact schisto - 1. Formulaire Village V3</t>
-  </si>
-  <si>
-    <t>bf_202301_sch_impact_assessment_1_sites_v3</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Région</t>
+  </si>
+  <si>
+    <t>District sanitaires</t>
+  </si>
+  <si>
+    <t>CM URBAIN</t>
+  </si>
+  <si>
+    <t>CSPS GODO</t>
+  </si>
+  <si>
+    <t>CSPS NAZOANGA</t>
+  </si>
+  <si>
+    <t>CSPS SOMASSI</t>
+  </si>
+  <si>
+    <t>CSPS SOAW</t>
+  </si>
+  <si>
+    <t>CSPS KINDI</t>
+  </si>
+  <si>
+    <t>CSPS NASSOULOU</t>
+  </si>
+  <si>
+    <t>CSPS KONE</t>
+  </si>
+  <si>
+    <t>CSPS LALLE</t>
+  </si>
+  <si>
+    <t>CSPS KOURIA</t>
+  </si>
+  <si>
+    <t>SAKOINSE</t>
+  </si>
+  <si>
+    <t>RAMONGO</t>
+  </si>
+  <si>
+    <t>PITMOAGA</t>
+  </si>
+  <si>
+    <t>CMK</t>
+  </si>
+  <si>
+    <t>PEHIRI</t>
+  </si>
+  <si>
+    <t>RANA</t>
+  </si>
+  <si>
+    <t>SOME</t>
+  </si>
+  <si>
+    <t>BINGO</t>
+  </si>
+  <si>
+    <t>IMASGO</t>
+  </si>
+  <si>
+    <t>BANABA</t>
+  </si>
+  <si>
+    <t>BATIE</t>
+  </si>
+  <si>
+    <t>BOPIEL</t>
+  </si>
+  <si>
+    <t>DANKANA</t>
+  </si>
+  <si>
+    <t>FADIO</t>
+  </si>
+  <si>
+    <t>KORIBA</t>
+  </si>
+  <si>
+    <t>LEGMOIN</t>
+  </si>
+  <si>
+    <t>MIDEBDO</t>
+  </si>
+  <si>
+    <t>KOUDJO</t>
+  </si>
+  <si>
+    <t>ZINDI</t>
+  </si>
+  <si>
+    <t>BILBALE</t>
+  </si>
+  <si>
+    <t>DADONE</t>
+  </si>
+  <si>
+    <t>DISSIHN</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>KOKOLIBOU</t>
+  </si>
+  <si>
+    <t>KPOPERI</t>
+  </si>
+  <si>
+    <t>MOU</t>
+  </si>
+  <si>
+    <t>NAKAR</t>
+  </si>
+  <si>
+    <t>NAMARE</t>
+  </si>
+  <si>
+    <t>NAVRIKPE</t>
+  </si>
+  <si>
+    <t>BANA</t>
+  </si>
+  <si>
+    <t>KAHIN</t>
+  </si>
+  <si>
+    <t>KABOUROU</t>
+  </si>
+  <si>
+    <t>MAMOU</t>
+  </si>
+  <si>
+    <t>OUAHABOU</t>
+  </si>
+  <si>
+    <t>POMPOÏ</t>
+  </si>
+  <si>
+    <t>SIBY</t>
+  </si>
+  <si>
+    <t>TONE</t>
+  </si>
+  <si>
+    <t>VY</t>
+  </si>
+  <si>
+    <t>NANORO</t>
+  </si>
+  <si>
+    <t>KOUDOUGOU</t>
+  </si>
+  <si>
+    <t>BATIÉ</t>
+  </si>
+  <si>
+    <t>DANO</t>
+  </si>
+  <si>
+    <t>SIG NONGHIN</t>
+  </si>
+  <si>
+    <t>NOGR-MASSOM</t>
+  </si>
+  <si>
+    <t>BOROMO</t>
+  </si>
+  <si>
+    <t>BASSINKO</t>
+  </si>
+  <si>
+    <t>BISSIGHIN</t>
+  </si>
+  <si>
+    <t>KAMBOINCIN</t>
+  </si>
+  <si>
+    <t>COOPERATION ALLEMANDE</t>
+  </si>
+  <si>
+    <t>CSPS BILGO</t>
+  </si>
+  <si>
+    <t>CSPS GOUPANA</t>
+  </si>
+  <si>
+    <t>CSPS NEDOGO</t>
+  </si>
+  <si>
+    <t>CSPS SAINT JOSEPH</t>
+  </si>
+  <si>
+    <t>CSPS SABTENGA</t>
+  </si>
+  <si>
+    <t>ZIBAKO</t>
+  </si>
+  <si>
+    <t>BANPORÉ</t>
+  </si>
+  <si>
+    <t>POLESGO</t>
+  </si>
+  <si>
+    <t>ROUMTENGA</t>
+  </si>
+  <si>
+    <t>SAKOULA</t>
+  </si>
+  <si>
+    <t>SECTEUR 13</t>
+  </si>
+  <si>
+    <t>SECTEUR 23</t>
+  </si>
+  <si>
+    <t>SECTEUR 25</t>
+  </si>
+  <si>
+    <t>SECTEUR 26</t>
+  </si>
+  <si>
+    <t>SECTEUR 27</t>
+  </si>
+  <si>
+    <t>SOGDIN</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>CENTRE-OUEST</t>
+  </si>
+  <si>
+    <t>SUD-OUEST</t>
+  </si>
+  <si>
+    <t>CENTRE</t>
+  </si>
+  <si>
+    <t>BOUCLE DU MOUHOUN</t>
+  </si>
+  <si>
+    <t>bf_202305_sch_impact_assessment_1_sites</t>
+  </si>
+  <si>
+    <t>(BF - Mai 2023) impact schisto - 1. Formulaire Village</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -966,8 +972,29 @@
       <name val="Arial"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -989,6 +1016,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1020,7 +1053,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1060,11 +1093,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2252,13 +2310,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11:XFD92"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24:E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -2388,10 +2446,10 @@
         <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>285</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2399,10 +2457,10 @@
         <v>95</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>284</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>109</v>
+        <v>284</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2414,45 +2472,46 @@
         <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>110</v>
+        <v>282</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>110</v>
+        <v>282</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" s="3" customFormat="1">
-      <c r="A14" s="6"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" t="s">
-        <v>108</v>
-      </c>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1">
+      <c r="A15" s="6"/>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -2460,13 +2519,13 @@
         <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>113</v>
+        <v>259</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>109</v>
+        <v>259</v>
+      </c>
+      <c r="D17" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -2474,13 +2533,13 @@
         <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>114</v>
+        <v>258</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>258</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>109</v>
+        <v>284</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -2488,13 +2547,13 @@
         <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>109</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -2502,13 +2561,13 @@
         <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2516,46 +2575,44 @@
         <v>96</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>256</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>256</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="3" customFormat="1">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-      <c r="C23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" t="s">
-        <v>111</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>257</v>
+      </c>
+      <c r="C22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="3" customFormat="1">
+      <c r="A23" s="6"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="E24" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -2565,13 +2622,13 @@
         <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>121</v>
+        <v>226</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>226</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -2581,13 +2638,13 @@
         <v>97</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>227</v>
       </c>
       <c r="E26" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -2597,13 +2654,13 @@
         <v>97</v>
       </c>
       <c r="B27" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>228</v>
       </c>
       <c r="E27" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -2613,13 +2670,13 @@
         <v>97</v>
       </c>
       <c r="B28" t="s">
-        <v>126</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>126</v>
+        <v>229</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -2629,13 +2686,13 @@
         <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -2645,13 +2702,13 @@
         <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="E30" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -2661,13 +2718,13 @@
         <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>130</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
-        <v>130</v>
+        <v>231</v>
       </c>
       <c r="E31" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2677,13 +2734,13 @@
         <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
       <c r="C32" t="s">
-        <v>132</v>
+        <v>232</v>
       </c>
       <c r="E32" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -2693,13 +2750,13 @@
         <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>133</v>
+        <v>234</v>
       </c>
       <c r="C33" t="s">
-        <v>134</v>
+        <v>234</v>
       </c>
       <c r="E33" t="s">
-        <v>112</v>
+        <v>256</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -2709,13 +2766,13 @@
         <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="C34" t="s">
-        <v>135</v>
+        <v>245</v>
       </c>
       <c r="E34" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
@@ -2725,13 +2782,13 @@
         <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
+        <v>247</v>
       </c>
       <c r="E35" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -2741,13 +2798,13 @@
         <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>246</v>
       </c>
       <c r="E36" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -2757,13 +2814,13 @@
         <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="C37" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2773,13 +2830,13 @@
         <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>139</v>
+        <v>249</v>
       </c>
       <c r="C38" t="s">
-        <v>140</v>
+        <v>249</v>
       </c>
       <c r="E38" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
@@ -2789,13 +2846,13 @@
         <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>141</v>
+        <v>281</v>
       </c>
       <c r="C39" t="s">
-        <v>141</v>
+        <v>281</v>
       </c>
       <c r="E39" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
@@ -2805,13 +2862,13 @@
         <v>97</v>
       </c>
       <c r="B40" t="s">
-        <v>142</v>
+        <v>250</v>
       </c>
       <c r="C40" t="s">
-        <v>142</v>
+        <v>250</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
@@ -2821,13 +2878,13 @@
         <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>143</v>
+        <v>251</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>251</v>
       </c>
       <c r="E41" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
@@ -2837,13 +2894,13 @@
         <v>97</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>252</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>252</v>
       </c>
       <c r="E42" t="s">
-        <v>112</v>
+        <v>260</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
@@ -2853,13 +2910,13 @@
         <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>253</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>253</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
+        <v>260</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
@@ -2869,13 +2926,13 @@
         <v>97</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>235</v>
       </c>
       <c r="C44" t="s">
-        <v>146</v>
+        <v>235</v>
       </c>
       <c r="E44" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7"/>
@@ -2885,13 +2942,13 @@
         <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>147</v>
+        <v>236</v>
       </c>
       <c r="C45" t="s">
-        <v>147</v>
+        <v>236</v>
       </c>
       <c r="E45" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
@@ -2901,13 +2958,13 @@
         <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>148</v>
+        <v>237</v>
       </c>
       <c r="C46" t="s">
-        <v>148</v>
+        <v>237</v>
       </c>
       <c r="E46" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
@@ -2917,13 +2974,13 @@
         <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>149</v>
+        <v>238</v>
       </c>
       <c r="C47" t="s">
-        <v>149</v>
+        <v>238</v>
       </c>
       <c r="E47" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
@@ -2933,13 +2990,13 @@
         <v>97</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>239</v>
       </c>
       <c r="C48" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="E48" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
@@ -2949,13 +3006,13 @@
         <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="C49" t="s">
-        <v>152</v>
+        <v>240</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7"/>
@@ -2965,13 +3022,13 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>153</v>
+        <v>241</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>241</v>
       </c>
       <c r="E50" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7"/>
@@ -2981,13 +3038,13 @@
         <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="C51" t="s">
-        <v>154</v>
+        <v>242</v>
       </c>
       <c r="E51" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7"/>
@@ -2997,13 +3054,13 @@
         <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>243</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>243</v>
       </c>
       <c r="E52" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
@@ -3013,13 +3070,13 @@
         <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>156</v>
+        <v>244</v>
       </c>
       <c r="C53" t="s">
-        <v>156</v>
+        <v>244</v>
       </c>
       <c r="E53" t="s">
-        <v>115</v>
+        <v>257</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
@@ -3029,13 +3086,13 @@
         <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="C54" t="s">
-        <v>156</v>
+        <v>223</v>
       </c>
       <c r="E54" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="7"/>
@@ -3045,13 +3102,13 @@
         <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="E55" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
@@ -3061,13 +3118,13 @@
         <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="C56" t="s">
-        <v>158</v>
+        <v>219</v>
       </c>
       <c r="E56" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
@@ -3077,13 +3134,13 @@
         <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="C57" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
@@ -3093,13 +3150,13 @@
         <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="C58" t="s">
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="E58" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7"/>
@@ -3109,13 +3166,13 @@
         <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>218</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7"/>
@@ -3125,13 +3182,13 @@
         <v>97</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
       <c r="E60" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
@@ -3141,13 +3198,13 @@
         <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="C61" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
@@ -3157,13 +3214,13 @@
         <v>97</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="C62" t="s">
-        <v>163</v>
+        <v>216</v>
       </c>
       <c r="E62" t="s">
-        <v>115</v>
+        <v>255</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
@@ -3173,13 +3230,13 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="C63" t="s">
-        <v>164</v>
+        <v>222</v>
       </c>
       <c r="E63" t="s">
-        <v>114</v>
+        <v>255</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7"/>
@@ -3189,13 +3246,13 @@
         <v>97</v>
       </c>
       <c r="B64" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="C64" t="s">
-        <v>165</v>
+        <v>206</v>
       </c>
       <c r="E64" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
@@ -3205,13 +3262,13 @@
         <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="E65" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -3221,13 +3278,13 @@
         <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>211</v>
       </c>
       <c r="E66" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
@@ -3237,13 +3294,13 @@
         <v>97</v>
       </c>
       <c r="B67" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>213</v>
       </c>
       <c r="E67" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="7"/>
@@ -3253,13 +3310,13 @@
         <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>215</v>
       </c>
       <c r="E68" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
@@ -3269,13 +3326,13 @@
         <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="C69" t="s">
-        <v>170</v>
+        <v>214</v>
       </c>
       <c r="E69" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7"/>
@@ -3285,13 +3342,13 @@
         <v>97</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="E70" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
@@ -3301,13 +3358,13 @@
         <v>97</v>
       </c>
       <c r="B71" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="C71" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
       <c r="E71" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -3317,13 +3374,13 @@
         <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="C72" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
       <c r="E72" t="s">
-        <v>114</v>
+        <v>254</v>
       </c>
       <c r="F72" s="7"/>
       <c r="G72" s="7"/>
@@ -3333,13 +3390,13 @@
         <v>97</v>
       </c>
       <c r="B73" t="s">
-        <v>284</v>
+        <v>209</v>
       </c>
       <c r="C73" t="s">
-        <v>284</v>
+        <v>209</v>
       </c>
       <c r="E73" t="s">
-        <v>116</v>
+        <v>254</v>
       </c>
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
@@ -3349,13 +3406,13 @@
         <v>97</v>
       </c>
       <c r="B74" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C74" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="E74" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
@@ -3365,13 +3422,13 @@
         <v>97</v>
       </c>
       <c r="B75" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="E75" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -3381,13 +3438,13 @@
         <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>175</v>
+        <v>273</v>
       </c>
       <c r="C76" t="s">
-        <v>175</v>
+        <v>273</v>
       </c>
       <c r="E76" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
@@ -3397,13 +3454,13 @@
         <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>176</v>
+        <v>274</v>
       </c>
       <c r="C77" t="s">
-        <v>176</v>
+        <v>274</v>
       </c>
       <c r="E77" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
@@ -3413,13 +3470,13 @@
         <v>97</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C78" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E78" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -3429,13 +3486,13 @@
         <v>97</v>
       </c>
       <c r="B79" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C79" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="E79" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -3445,13 +3502,13 @@
         <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>177</v>
+        <v>277</v>
       </c>
       <c r="C80" t="s">
-        <v>177</v>
+        <v>277</v>
       </c>
       <c r="E80" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
@@ -3461,13 +3518,13 @@
         <v>97</v>
       </c>
       <c r="B81" t="s">
-        <v>178</v>
+        <v>278</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>278</v>
       </c>
       <c r="E81" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
@@ -3477,13 +3534,13 @@
         <v>97</v>
       </c>
       <c r="B82" t="s">
-        <v>179</v>
+        <v>279</v>
       </c>
       <c r="C82" t="s">
-        <v>179</v>
+        <v>279</v>
       </c>
       <c r="E82" t="s">
-        <v>116</v>
+        <v>259</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7"/>
@@ -3493,13 +3550,13 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>180</v>
+        <v>280</v>
       </c>
       <c r="C83" t="s">
-        <v>180</v>
+        <v>280</v>
       </c>
       <c r="E83" t="s">
-        <v>117</v>
+        <v>259</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -3509,13 +3566,13 @@
         <v>97</v>
       </c>
       <c r="B84" t="s">
-        <v>181</v>
+        <v>261</v>
       </c>
       <c r="C84" t="s">
-        <v>181</v>
+        <v>261</v>
       </c>
       <c r="E84" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -3525,13 +3582,13 @@
         <v>97</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>262</v>
       </c>
       <c r="C85" t="s">
-        <v>182</v>
+        <v>262</v>
       </c>
       <c r="E85" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -3541,13 +3598,13 @@
         <v>97</v>
       </c>
       <c r="B86" t="s">
-        <v>183</v>
+        <v>264</v>
       </c>
       <c r="C86" t="s">
-        <v>183</v>
+        <v>264</v>
       </c>
       <c r="E86" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7"/>
@@ -3557,13 +3614,13 @@
         <v>97</v>
       </c>
       <c r="B87" t="s">
-        <v>184</v>
+        <v>265</v>
       </c>
       <c r="C87" t="s">
-        <v>184</v>
+        <v>265</v>
       </c>
       <c r="E87" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
@@ -3573,13 +3630,13 @@
         <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
       <c r="C88" t="s">
-        <v>185</v>
+        <v>266</v>
       </c>
       <c r="E88" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -3589,13 +3646,13 @@
         <v>97</v>
       </c>
       <c r="B89" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="C89" t="s">
-        <v>186</v>
+        <v>267</v>
       </c>
       <c r="E89" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
@@ -3605,13 +3662,13 @@
         <v>97</v>
       </c>
       <c r="B90" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
       <c r="C90" t="s">
-        <v>187</v>
+        <v>269</v>
       </c>
       <c r="E90" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -3621,13 +3678,13 @@
         <v>97</v>
       </c>
       <c r="B91" t="s">
-        <v>188</v>
+        <v>268</v>
       </c>
       <c r="C91" t="s">
-        <v>188</v>
+        <v>268</v>
       </c>
       <c r="E91" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -3637,600 +3694,616 @@
         <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>189</v>
+        <v>263</v>
       </c>
       <c r="C92" t="s">
-        <v>189</v>
+        <v>263</v>
       </c>
       <c r="E92" t="s">
-        <v>117</v>
+        <v>258</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
     </row>
-    <row r="93" spans="1:7" s="3" customFormat="1">
-      <c r="A93" s="6"/>
-    </row>
-    <row r="94" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A94" t="s">
-        <v>190</v>
-      </c>
-      <c r="B94" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" t="s">
+        <v>270</v>
+      </c>
+      <c r="C93" t="s">
+        <v>270</v>
+      </c>
+      <c r="E93" t="s">
+        <v>258</v>
+      </c>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94" spans="1:7" s="3" customFormat="1">
+      <c r="A94" s="6"/>
+    </row>
+    <row r="95" spans="1:7" ht="15.75" customHeight="1">
       <c r="A95" t="s">
-        <v>190</v>
-      </c>
-      <c r="B95" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" s="3" customFormat="1">
-      <c r="A96" s="6"/>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>193</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>195</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>109</v>
+      </c>
+      <c r="B96" t="s">
+        <v>111</v>
+      </c>
+      <c r="C96" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="3" customFormat="1">
+      <c r="A97" s="6"/>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>193</v>
-      </c>
-      <c r="B98" t="s">
-        <v>196</v>
-      </c>
-      <c r="C98" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" s="3" customFormat="1"/>
-    <row r="100" spans="1:7">
-      <c r="A100" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B100" t="s">
-        <v>199</v>
-      </c>
-      <c r="C100" t="s">
-        <v>200</v>
-      </c>
-      <c r="G100" s="7"/>
-    </row>
+        <v>112</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>112</v>
+      </c>
+      <c r="B99" t="s">
+        <v>115</v>
+      </c>
+      <c r="C99" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="3" customFormat="1"/>
     <row r="101" spans="1:7">
       <c r="A101" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B101" t="s">
-        <v>201</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>202</v>
+        <v>119</v>
       </c>
       <c r="G101" s="7"/>
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B102" t="s">
-        <v>203</v>
+        <v>120</v>
       </c>
       <c r="C102" t="s">
-        <v>204</v>
+        <v>121</v>
       </c>
       <c r="G102" s="7"/>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B103" t="s">
-        <v>205</v>
+        <v>122</v>
       </c>
       <c r="C103" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="G103" s="7"/>
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>208</v>
+        <v>117</v>
+      </c>
+      <c r="B104" t="s">
+        <v>124</v>
+      </c>
+      <c r="C104" t="s">
+        <v>125</v>
       </c>
       <c r="G104" s="7"/>
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B105" t="s">
-        <v>209</v>
-      </c>
-      <c r="C105" t="s">
-        <v>210</v>
+        <v>117</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="G105" s="7"/>
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>128</v>
       </c>
       <c r="C106" t="s">
-        <v>212</v>
+        <v>129</v>
       </c>
       <c r="G106" s="7"/>
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B107" t="s">
-        <v>213</v>
+        <v>130</v>
       </c>
       <c r="C107" t="s">
-        <v>214</v>
+        <v>131</v>
       </c>
       <c r="G107" s="7"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B108" t="s">
-        <v>215</v>
+        <v>132</v>
       </c>
       <c r="C108" t="s">
-        <v>216</v>
+        <v>133</v>
       </c>
       <c r="G108" s="7"/>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B109" t="s">
-        <v>217</v>
+        <v>134</v>
       </c>
       <c r="C109" t="s">
-        <v>218</v>
+        <v>135</v>
       </c>
       <c r="G109" s="7"/>
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B110" t="s">
-        <v>219</v>
+        <v>136</v>
       </c>
       <c r="C110" t="s">
-        <v>220</v>
+        <v>137</v>
       </c>
       <c r="G110" s="7"/>
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="1" t="s">
-        <v>198</v>
+        <v>117</v>
       </c>
       <c r="B111" t="s">
-        <v>221</v>
+        <v>138</v>
       </c>
       <c r="C111" t="s">
-        <v>221</v>
+        <v>139</v>
       </c>
       <c r="G111" s="7"/>
     </row>
-    <row r="112" spans="1:7" s="3" customFormat="1">
-      <c r="A112" s="6"/>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>195</v>
-      </c>
+    <row r="112" spans="1:7">
+      <c r="A112" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B112" t="s">
+        <v>140</v>
+      </c>
+      <c r="C112" t="s">
+        <v>140</v>
+      </c>
+      <c r="G112" s="7"/>
+    </row>
+    <row r="113" spans="1:3" s="3" customFormat="1">
+      <c r="A113" s="6"/>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B114" t="s">
-        <v>223</v>
-      </c>
-      <c r="C114" t="s">
-        <v>224</v>
+        <v>141</v>
+      </c>
+      <c r="B114" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C114" s="8" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
-        <v>222</v>
+        <v>141</v>
       </c>
       <c r="B115" t="s">
-        <v>225</v>
+        <v>142</v>
       </c>
       <c r="C115" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" s="3" customFormat="1">
-      <c r="A116" s="6"/>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B117" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="C117" s="9" t="s">
-        <v>229</v>
-      </c>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B116" t="s">
+        <v>144</v>
+      </c>
+      <c r="C116" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" s="3" customFormat="1">
+      <c r="A117" s="6"/>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>230</v>
+        <v>147</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>231</v>
+        <v>148</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>232</v>
+        <v>149</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>233</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
-        <v>227</v>
+        <v>146</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>234</v>
+        <v>151</v>
       </c>
       <c r="C120" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" s="3" customFormat="1">
-      <c r="A121" s="6"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>237</v>
-      </c>
-      <c r="C122" s="9" t="s">
-        <v>238</v>
-      </c>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C121" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" s="3" customFormat="1">
+      <c r="A122" s="6"/>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
-        <v>236</v>
+        <v>155</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>239</v>
+        <v>156</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>240</v>
+        <v>157</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
-        <v>236</v>
+        <v>155</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>242</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="1" t="s">
-        <v>236</v>
+        <v>155</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>243</v>
+        <v>160</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>244</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
-        <v>236</v>
+        <v>155</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>245</v>
+        <v>162</v>
       </c>
       <c r="C126" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" s="3" customFormat="1">
-      <c r="A127" s="6"/>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
-        <v>247</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="C128" s="9" t="s">
-        <v>249</v>
-      </c>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C127" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" s="3" customFormat="1">
+      <c r="A128" s="6"/>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>247</v>
+        <v>166</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>250</v>
+        <v>167</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>251</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>247</v>
+        <v>166</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>252</v>
+        <v>169</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>253</v>
+        <v>170</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>247</v>
+        <v>166</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>254</v>
+        <v>171</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>255</v>
+        <v>172</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>247</v>
+        <v>166</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>256</v>
+        <v>173</v>
       </c>
       <c r="C132" s="9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" s="3" customFormat="1">
-      <c r="A133" s="6"/>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>258</v>
-      </c>
-      <c r="B134" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="C134" s="10" t="s">
-        <v>260</v>
-      </c>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>166</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" s="3" customFormat="1">
+      <c r="A134" s="6"/>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>258</v>
+        <v>177</v>
       </c>
       <c r="B135" s="10" t="s">
-        <v>261</v>
+        <v>178</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>261</v>
+        <v>179</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>177</v>
       </c>
       <c r="B136" s="10" t="s">
-        <v>262</v>
+        <v>180</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>263</v>
+        <v>180</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>258</v>
+        <v>177</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>264</v>
+        <v>181</v>
       </c>
       <c r="C137" s="10" t="s">
-        <v>265</v>
+        <v>182</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>258</v>
+        <v>177</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>266</v>
+        <v>183</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" s="3" customFormat="1">
-      <c r="A139" s="6"/>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>268</v>
-      </c>
-      <c r="B140" s="10" t="s">
-        <v>269</v>
-      </c>
-      <c r="C140" s="10" t="s">
-        <v>269</v>
-      </c>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>177</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" s="3" customFormat="1">
+      <c r="A140" s="6"/>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B141" s="10" t="s">
-        <v>270</v>
+        <v>188</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>271</v>
+        <v>188</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>272</v>
+        <v>189</v>
       </c>
       <c r="C142" s="10" t="s">
-        <v>272</v>
+        <v>190</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B143" s="10" t="s">
-        <v>273</v>
+        <v>191</v>
       </c>
       <c r="C143" s="10" t="s">
-        <v>274</v>
+        <v>191</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B144" s="10" t="s">
-        <v>275</v>
+        <v>192</v>
       </c>
       <c r="C144" s="10" t="s">
-        <v>276</v>
+        <v>193</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>268</v>
+        <v>187</v>
       </c>
       <c r="B145" s="10" t="s">
-        <v>277</v>
+        <v>194</v>
       </c>
       <c r="C145" s="10" t="s">
-        <v>278</v>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>187</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C146" s="10" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A42:G56">
-    <sortCondition ref="B42:B56"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A43:G57">
+    <sortCondition ref="B43:B57"/>
   </sortState>
-  <conditionalFormatting sqref="E109">
-    <cfRule type="duplicateValues" dxfId="25" priority="81"/>
+  <conditionalFormatting sqref="E110">
+    <cfRule type="duplicateValues" dxfId="27" priority="81"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="duplicateValues" dxfId="24" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="16"/>
+  <conditionalFormatting sqref="C112">
+    <cfRule type="duplicateValues" dxfId="26" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G115">
-    <cfRule type="duplicateValues" dxfId="22" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="31"/>
+  <conditionalFormatting sqref="G116">
+    <cfRule type="duplicateValues" dxfId="24" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
-    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="12"/>
+  <conditionalFormatting sqref="B117">
+    <cfRule type="duplicateValues" dxfId="22" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F119">
-    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
+  <conditionalFormatting sqref="F120">
+    <cfRule type="duplicateValues" dxfId="20" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B121">
-    <cfRule type="duplicateValues" dxfId="17" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="10"/>
+  <conditionalFormatting sqref="B122">
+    <cfRule type="duplicateValues" dxfId="19" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F122">
-    <cfRule type="duplicateValues" dxfId="15" priority="19"/>
+  <conditionalFormatting sqref="F123">
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124">
-    <cfRule type="duplicateValues" dxfId="14" priority="27"/>
+  <conditionalFormatting sqref="E125">
+    <cfRule type="duplicateValues" dxfId="16" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B127">
-    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="8"/>
+  <conditionalFormatting sqref="B128">
+    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G128">
-    <cfRule type="duplicateValues" dxfId="11" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="26"/>
+  <conditionalFormatting sqref="G129">
+    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B133">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+  <conditionalFormatting sqref="B134">
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B139">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+  <conditionalFormatting sqref="B140">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B100:B112">
-    <cfRule type="duplicateValues" dxfId="5" priority="96"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="97"/>
+  <conditionalFormatting sqref="B101:B113">
+    <cfRule type="duplicateValues" dxfId="7" priority="96"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="97"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100:C110">
-    <cfRule type="duplicateValues" dxfId="3" priority="102"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="103"/>
+  <conditionalFormatting sqref="C101:C111">
+    <cfRule type="duplicateValues" dxfId="5" priority="102"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="103"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G124:G125">
-    <cfRule type="duplicateValues" dxfId="1" priority="33"/>
+  <conditionalFormatting sqref="G125:G126">
+    <cfRule type="duplicateValues" dxfId="3" priority="33"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G115 G122:G126 G117:G120">
-    <cfRule type="duplicateValues" dxfId="0" priority="95"/>
+  <conditionalFormatting sqref="G116 G123:G127 G118:G121">
+    <cfRule type="duplicateValues" dxfId="2" priority="95"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4241,8 +4314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75"/>
@@ -4253,33 +4326,1554 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
-        <v>281</v>
+        <v>200</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>282</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>288</v>
+      <c r="A2" s="19" t="s">
+        <v>287</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>283</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB163701-A23A-4287-9ABE-ADE1596168A2}">
+  <dimension ref="A1:M71"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="18" customFormat="1">
+      <c r="A1" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G2" t="s">
+        <v>285</v>
+      </c>
+      <c r="I2" t="s">
+        <v>285</v>
+      </c>
+      <c r="J2" t="s">
+        <v>260</v>
+      </c>
+      <c r="L2" t="s">
+        <v>256</v>
+      </c>
+      <c r="M2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="G3" t="s">
+        <v>284</v>
+      </c>
+      <c r="I3" t="s">
+        <v>284</v>
+      </c>
+      <c r="J3" t="s">
+        <v>259</v>
+      </c>
+      <c r="L3" t="s">
+        <v>256</v>
+      </c>
+      <c r="M3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>282</v>
+      </c>
+      <c r="C4" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G4" t="s">
+        <v>282</v>
+      </c>
+      <c r="I4" t="s">
+        <v>284</v>
+      </c>
+      <c r="J4" t="s">
+        <v>258</v>
+      </c>
+      <c r="L4" t="s">
+        <v>256</v>
+      </c>
+      <c r="M4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G5" t="s">
+        <v>283</v>
+      </c>
+      <c r="I5" t="s">
+        <v>282</v>
+      </c>
+      <c r="J5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L5" t="s">
+        <v>256</v>
+      </c>
+      <c r="M5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" t="s">
+        <v>210</v>
+      </c>
+      <c r="I6" t="s">
+        <v>282</v>
+      </c>
+      <c r="J6" t="s">
+        <v>254</v>
+      </c>
+      <c r="L6" t="s">
+        <v>256</v>
+      </c>
+      <c r="M6" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" t="s">
+        <v>283</v>
+      </c>
+      <c r="J7" t="s">
+        <v>256</v>
+      </c>
+      <c r="L7" t="s">
+        <v>256</v>
+      </c>
+      <c r="M7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" t="s">
+        <v>212</v>
+      </c>
+      <c r="I8" t="s">
+        <v>283</v>
+      </c>
+      <c r="J8" t="s">
+        <v>257</v>
+      </c>
+      <c r="L8" t="s">
+        <v>256</v>
+      </c>
+      <c r="M8" s="17" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" t="s">
+        <v>213</v>
+      </c>
+      <c r="L9" t="s">
+        <v>256</v>
+      </c>
+      <c r="M9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>282</v>
+      </c>
+      <c r="C10" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" t="s">
+        <v>214</v>
+      </c>
+      <c r="L10" t="s">
+        <v>256</v>
+      </c>
+      <c r="M10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
+        <v>215</v>
+      </c>
+      <c r="L11" t="s">
+        <v>256</v>
+      </c>
+      <c r="M11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L12" t="s">
+        <v>260</v>
+      </c>
+      <c r="M12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>282</v>
+      </c>
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" t="s">
+        <v>217</v>
+      </c>
+      <c r="L13" t="s">
+        <v>260</v>
+      </c>
+      <c r="M13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" t="s">
+        <v>255</v>
+      </c>
+      <c r="D14" t="s">
+        <v>218</v>
+      </c>
+      <c r="L14" t="s">
+        <v>260</v>
+      </c>
+      <c r="M14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>282</v>
+      </c>
+      <c r="C15" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" t="s">
+        <v>219</v>
+      </c>
+      <c r="L15" t="s">
+        <v>260</v>
+      </c>
+      <c r="M15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D16" t="s">
+        <v>220</v>
+      </c>
+      <c r="L16" t="s">
+        <v>260</v>
+      </c>
+      <c r="M16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>282</v>
+      </c>
+      <c r="C17" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" t="s">
+        <v>221</v>
+      </c>
+      <c r="L17" t="s">
+        <v>260</v>
+      </c>
+      <c r="M17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>282</v>
+      </c>
+      <c r="C18" t="s">
+        <v>255</v>
+      </c>
+      <c r="D18" t="s">
+        <v>222</v>
+      </c>
+      <c r="L18" t="s">
+        <v>260</v>
+      </c>
+      <c r="M18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>282</v>
+      </c>
+      <c r="C19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" t="s">
+        <v>223</v>
+      </c>
+      <c r="L19" t="s">
+        <v>260</v>
+      </c>
+      <c r="M19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>282</v>
+      </c>
+      <c r="C20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" t="s">
+        <v>224</v>
+      </c>
+      <c r="L20" t="s">
+        <v>260</v>
+      </c>
+      <c r="M20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" t="s">
+        <v>255</v>
+      </c>
+      <c r="D21" t="s">
+        <v>108</v>
+      </c>
+      <c r="L21" t="s">
+        <v>260</v>
+      </c>
+      <c r="M21" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" t="s">
+        <v>225</v>
+      </c>
+      <c r="L22" t="s">
+        <v>257</v>
+      </c>
+      <c r="M22" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" t="s">
+        <v>256</v>
+      </c>
+      <c r="D23" t="s">
+        <v>226</v>
+      </c>
+      <c r="L23" t="s">
+        <v>257</v>
+      </c>
+      <c r="M23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" t="s">
+        <v>227</v>
+      </c>
+      <c r="L24" t="s">
+        <v>257</v>
+      </c>
+      <c r="M24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>283</v>
+      </c>
+      <c r="C25" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" t="s">
+        <v>228</v>
+      </c>
+      <c r="L25" t="s">
+        <v>257</v>
+      </c>
+      <c r="M25" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>283</v>
+      </c>
+      <c r="C26" t="s">
+        <v>256</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="L26" t="s">
+        <v>257</v>
+      </c>
+      <c r="M26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C27" t="s">
+        <v>256</v>
+      </c>
+      <c r="D27" t="s">
+        <v>230</v>
+      </c>
+      <c r="L27" t="s">
+        <v>257</v>
+      </c>
+      <c r="M27" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>283</v>
+      </c>
+      <c r="C28" t="s">
+        <v>256</v>
+      </c>
+      <c r="D28" t="s">
+        <v>231</v>
+      </c>
+      <c r="L28" t="s">
+        <v>257</v>
+      </c>
+      <c r="M28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>283</v>
+      </c>
+      <c r="C29" t="s">
+        <v>256</v>
+      </c>
+      <c r="D29" t="s">
+        <v>232</v>
+      </c>
+      <c r="L29" t="s">
+        <v>257</v>
+      </c>
+      <c r="M29" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C30" t="s">
+        <v>256</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="L30" t="s">
+        <v>257</v>
+      </c>
+      <c r="M30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>283</v>
+      </c>
+      <c r="C31" t="s">
+        <v>256</v>
+      </c>
+      <c r="D31" t="s">
+        <v>234</v>
+      </c>
+      <c r="L31" t="s">
+        <v>257</v>
+      </c>
+      <c r="M31" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>283</v>
+      </c>
+      <c r="C32" t="s">
+        <v>257</v>
+      </c>
+      <c r="D32" t="s">
+        <v>235</v>
+      </c>
+      <c r="L32" t="s">
+        <v>255</v>
+      </c>
+      <c r="M32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>283</v>
+      </c>
+      <c r="C33" t="s">
+        <v>257</v>
+      </c>
+      <c r="D33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L33" t="s">
+        <v>255</v>
+      </c>
+      <c r="M33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>283</v>
+      </c>
+      <c r="C34" t="s">
+        <v>257</v>
+      </c>
+      <c r="D34" t="s">
+        <v>237</v>
+      </c>
+      <c r="L34" t="s">
+        <v>255</v>
+      </c>
+      <c r="M34" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>283</v>
+      </c>
+      <c r="C35" t="s">
+        <v>257</v>
+      </c>
+      <c r="D35" t="s">
+        <v>238</v>
+      </c>
+      <c r="L35" t="s">
+        <v>255</v>
+      </c>
+      <c r="M35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" t="s">
+        <v>257</v>
+      </c>
+      <c r="D36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>255</v>
+      </c>
+      <c r="M36" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>283</v>
+      </c>
+      <c r="C37" t="s">
+        <v>257</v>
+      </c>
+      <c r="D37" t="s">
+        <v>240</v>
+      </c>
+      <c r="L37" t="s">
+        <v>255</v>
+      </c>
+      <c r="M37" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>283</v>
+      </c>
+      <c r="C38" t="s">
+        <v>257</v>
+      </c>
+      <c r="D38" t="s">
+        <v>241</v>
+      </c>
+      <c r="L38" t="s">
+        <v>255</v>
+      </c>
+      <c r="M38" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" t="s">
+        <v>257</v>
+      </c>
+      <c r="D39" t="s">
+        <v>242</v>
+      </c>
+      <c r="L39" t="s">
+        <v>255</v>
+      </c>
+      <c r="M39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" t="s">
+        <v>257</v>
+      </c>
+      <c r="D40" t="s">
+        <v>243</v>
+      </c>
+      <c r="L40" t="s">
+        <v>255</v>
+      </c>
+      <c r="M40" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C41" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" t="s">
+        <v>244</v>
+      </c>
+      <c r="L41" t="s">
+        <v>255</v>
+      </c>
+      <c r="M41" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>284</v>
+      </c>
+      <c r="C42" t="s">
+        <v>258</v>
+      </c>
+      <c r="D42" t="s">
+        <v>261</v>
+      </c>
+      <c r="L42" t="s">
+        <v>254</v>
+      </c>
+      <c r="M42" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C43" t="s">
+        <v>258</v>
+      </c>
+      <c r="D43" t="s">
+        <v>262</v>
+      </c>
+      <c r="L43" t="s">
+        <v>254</v>
+      </c>
+      <c r="M43" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44" t="s">
+        <v>284</v>
+      </c>
+      <c r="C44" t="s">
+        <v>258</v>
+      </c>
+      <c r="D44" t="s">
+        <v>263</v>
+      </c>
+      <c r="L44" t="s">
+        <v>254</v>
+      </c>
+      <c r="M44" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" t="s">
+        <v>264</v>
+      </c>
+      <c r="L45" t="s">
+        <v>254</v>
+      </c>
+      <c r="M45" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
+        <v>5</v>
+      </c>
+      <c r="B46" t="s">
+        <v>284</v>
+      </c>
+      <c r="C46" t="s">
+        <v>258</v>
+      </c>
+      <c r="D46" t="s">
+        <v>265</v>
+      </c>
+      <c r="L46" t="s">
+        <v>254</v>
+      </c>
+      <c r="M46" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>284</v>
+      </c>
+      <c r="C47" t="s">
+        <v>258</v>
+      </c>
+      <c r="D47" t="s">
+        <v>266</v>
+      </c>
+      <c r="L47" t="s">
+        <v>254</v>
+      </c>
+      <c r="M47" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>284</v>
+      </c>
+      <c r="C48" t="s">
+        <v>258</v>
+      </c>
+      <c r="D48" t="s">
+        <v>267</v>
+      </c>
+      <c r="L48" t="s">
+        <v>254</v>
+      </c>
+      <c r="M48" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49">
+        <v>8</v>
+      </c>
+      <c r="B49" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" t="s">
+        <v>258</v>
+      </c>
+      <c r="D49" t="s">
+        <v>268</v>
+      </c>
+      <c r="L49" t="s">
+        <v>254</v>
+      </c>
+      <c r="M49" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>284</v>
+      </c>
+      <c r="C50" t="s">
+        <v>258</v>
+      </c>
+      <c r="D50" t="s">
+        <v>269</v>
+      </c>
+      <c r="L50" t="s">
+        <v>254</v>
+      </c>
+      <c r="M50" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51">
+        <v>10</v>
+      </c>
+      <c r="B51" t="s">
+        <v>284</v>
+      </c>
+      <c r="C51" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" t="s">
+        <v>270</v>
+      </c>
+      <c r="L51" t="s">
+        <v>254</v>
+      </c>
+      <c r="M51" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
+        <v>284</v>
+      </c>
+      <c r="C52" t="s">
+        <v>259</v>
+      </c>
+      <c r="D52" t="s">
+        <v>271</v>
+      </c>
+      <c r="L52" t="s">
+        <v>259</v>
+      </c>
+      <c r="M52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" t="s">
+        <v>259</v>
+      </c>
+      <c r="D53" t="s">
+        <v>272</v>
+      </c>
+      <c r="L53" t="s">
+        <v>259</v>
+      </c>
+      <c r="M53" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54">
+        <v>3</v>
+      </c>
+      <c r="B54" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>259</v>
+      </c>
+      <c r="D54" t="s">
+        <v>273</v>
+      </c>
+      <c r="L54" t="s">
+        <v>259</v>
+      </c>
+      <c r="M54" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" t="s">
+        <v>259</v>
+      </c>
+      <c r="D55" t="s">
+        <v>274</v>
+      </c>
+      <c r="L55" t="s">
+        <v>259</v>
+      </c>
+      <c r="M55" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56" t="s">
+        <v>284</v>
+      </c>
+      <c r="C56" t="s">
+        <v>259</v>
+      </c>
+      <c r="D56" t="s">
+        <v>275</v>
+      </c>
+      <c r="L56" t="s">
+        <v>259</v>
+      </c>
+      <c r="M56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>284</v>
+      </c>
+      <c r="C57" t="s">
+        <v>259</v>
+      </c>
+      <c r="D57" t="s">
+        <v>276</v>
+      </c>
+      <c r="L57" t="s">
+        <v>259</v>
+      </c>
+      <c r="M57" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>284</v>
+      </c>
+      <c r="C58" t="s">
+        <v>259</v>
+      </c>
+      <c r="D58" t="s">
+        <v>277</v>
+      </c>
+      <c r="L58" t="s">
+        <v>259</v>
+      </c>
+      <c r="M58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59">
+        <v>8</v>
+      </c>
+      <c r="B59" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" t="s">
+        <v>259</v>
+      </c>
+      <c r="D59" t="s">
+        <v>278</v>
+      </c>
+      <c r="L59" t="s">
+        <v>259</v>
+      </c>
+      <c r="M59" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60">
+        <v>9</v>
+      </c>
+      <c r="B60" t="s">
+        <v>284</v>
+      </c>
+      <c r="C60" t="s">
+        <v>259</v>
+      </c>
+      <c r="D60" t="s">
+        <v>279</v>
+      </c>
+      <c r="L60" t="s">
+        <v>259</v>
+      </c>
+      <c r="M60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>284</v>
+      </c>
+      <c r="C61" t="s">
+        <v>259</v>
+      </c>
+      <c r="D61" t="s">
+        <v>280</v>
+      </c>
+      <c r="L61" t="s">
+        <v>259</v>
+      </c>
+      <c r="M61" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>285</v>
+      </c>
+      <c r="C62" t="s">
+        <v>260</v>
+      </c>
+      <c r="D62" t="s">
+        <v>245</v>
+      </c>
+      <c r="L62" t="s">
+        <v>258</v>
+      </c>
+      <c r="M62" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63" t="s">
+        <v>285</v>
+      </c>
+      <c r="C63" t="s">
+        <v>260</v>
+      </c>
+      <c r="D63" t="s">
+        <v>246</v>
+      </c>
+      <c r="L63" t="s">
+        <v>258</v>
+      </c>
+      <c r="M63" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64" t="s">
+        <v>285</v>
+      </c>
+      <c r="C64" t="s">
+        <v>260</v>
+      </c>
+      <c r="D64" t="s">
+        <v>247</v>
+      </c>
+      <c r="L64" t="s">
+        <v>258</v>
+      </c>
+      <c r="M64" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65" t="s">
+        <v>285</v>
+      </c>
+      <c r="C65" t="s">
+        <v>260</v>
+      </c>
+      <c r="D65" t="s">
+        <v>248</v>
+      </c>
+      <c r="L65" t="s">
+        <v>258</v>
+      </c>
+      <c r="M65" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66">
+        <v>5</v>
+      </c>
+      <c r="B66" t="s">
+        <v>285</v>
+      </c>
+      <c r="C66" t="s">
+        <v>260</v>
+      </c>
+      <c r="D66" t="s">
+        <v>249</v>
+      </c>
+      <c r="L66" t="s">
+        <v>258</v>
+      </c>
+      <c r="M66" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67" t="s">
+        <v>285</v>
+      </c>
+      <c r="C67" t="s">
+        <v>260</v>
+      </c>
+      <c r="D67" t="s">
+        <v>250</v>
+      </c>
+      <c r="L67" t="s">
+        <v>258</v>
+      </c>
+      <c r="M67" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>285</v>
+      </c>
+      <c r="C68" t="s">
+        <v>260</v>
+      </c>
+      <c r="D68" t="s">
+        <v>281</v>
+      </c>
+      <c r="L68" t="s">
+        <v>258</v>
+      </c>
+      <c r="M68" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>285</v>
+      </c>
+      <c r="C69" t="s">
+        <v>260</v>
+      </c>
+      <c r="D69" t="s">
+        <v>251</v>
+      </c>
+      <c r="L69" t="s">
+        <v>258</v>
+      </c>
+      <c r="M69" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>285</v>
+      </c>
+      <c r="C70" t="s">
+        <v>260</v>
+      </c>
+      <c r="D70" t="s">
+        <v>252</v>
+      </c>
+      <c r="L70" t="s">
+        <v>258</v>
+      </c>
+      <c r="M70" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71">
+        <v>10</v>
+      </c>
+      <c r="B71" t="s">
+        <v>285</v>
+      </c>
+      <c r="C71" t="s">
+        <v>260</v>
+      </c>
+      <c r="D71" t="s">
+        <v>253</v>
+      </c>
+      <c r="L71" t="s">
+        <v>258</v>
+      </c>
+      <c r="M71" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L2:M74">
+    <sortCondition ref="L2:L74"/>
+    <sortCondition ref="M2:M74"/>
+  </sortState>
+  <conditionalFormatting sqref="D1:D72 D75:D1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M1:M72 M75:M1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>